<commit_message>
Fixed Height in Name Field
</commit_message>
<xml_diff>
--- a/Salary Slip Data - Structure.xlsx
+++ b/Salary Slip Data - Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SalarySlipPDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE56BA8-31ED-4964-AB34-657A5BF616E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE76C02-06F2-4823-B966-07520C921985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,9 +608,6 @@
     <t>SEPTEMBER 2019</t>
   </si>
   <si>
-    <t>SARITADEVI C DHARIYA</t>
-  </si>
-  <si>
     <t>JAMILABIBI RAHIMKHAN BHUSHAVALA</t>
   </si>
   <si>
@@ -663,6 +660,9 @@
   </si>
   <si>
     <t>9876543210</t>
+  </si>
+  <si>
+    <t>SARITADEVI CHANDRIKAPRASAD DHARIYABCDEFGHIJKLMNOPQRSTUVWXYZ</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1038,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1124,7 @@
         <v>18</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>19</v>
@@ -1174,16 +1174,16 @@
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I2" s="6">
         <v>3285</v>
@@ -1263,13 +1263,13 @@
         <v>86</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I3" s="6">
         <v>3092</v>
@@ -1349,13 +1349,13 @@
         <v>87</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I4" s="6">
         <v>3463</v>
@@ -1435,13 +1435,13 @@
         <v>180</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I5" s="6">
         <v>3463</v>
@@ -1518,16 +1518,16 @@
         <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I6" s="6">
         <v>1536</v>
@@ -1607,13 +1607,13 @@
         <v>171</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I7" s="6">
         <v>4801</v>
@@ -1693,13 +1693,13 @@
         <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I8" s="6">
         <v>3073</v>
@@ -1779,13 +1779,13 @@
         <v>103</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I9" s="6">
         <v>15508</v>
@@ -1865,13 +1865,13 @@
         <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I10" s="6">
         <v>3285</v>
@@ -1951,13 +1951,13 @@
         <v>165</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I11" s="6">
         <v>2497</v>
@@ -2037,13 +2037,13 @@
         <v>110</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I12" s="6">
         <v>1920</v>
@@ -2114,22 +2114,22 @@
         <v>190</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I13" s="6">
         <v>192</v>
@@ -2209,13 +2209,13 @@
         <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I14" s="6">
         <v>2689</v>
@@ -2295,13 +2295,13 @@
         <v>88</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I15" s="6">
         <v>3073</v>
@@ -2381,13 +2381,13 @@
         <v>80</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I16" s="6">
         <v>3265</v>
@@ -2467,13 +2467,13 @@
         <v>43</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I17" s="6">
         <v>2112</v>
@@ -2550,16 +2550,16 @@
         <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I18" s="6">
         <v>5870</v>
@@ -2639,13 +2639,13 @@
         <v>123</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I19" s="6">
         <v>4831</v>
@@ -2725,13 +2725,13 @@
         <v>121</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I20" s="6">
         <v>14909</v>
@@ -2811,13 +2811,13 @@
         <v>130</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I21" s="6">
         <v>5506</v>
@@ -2897,13 +2897,13 @@
         <v>159</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I22" s="6">
         <v>12876</v>
@@ -2974,22 +2974,22 @@
         <v>190</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I23" s="6">
         <v>2386</v>
@@ -3069,13 +3069,13 @@
         <v>141</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I24" s="6">
         <v>5451</v>
@@ -3155,13 +3155,13 @@
         <v>139</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I25" s="6">
         <v>14118</v>
@@ -3241,13 +3241,13 @@
         <v>169</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I26" s="6">
         <v>4037</v>
@@ -3327,13 +3327,13 @@
         <v>161</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I27" s="6">
         <v>5266</v>
@@ -3413,13 +3413,13 @@
         <v>127</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I28" s="6">
         <v>6883</v>
@@ -3499,13 +3499,13 @@
         <v>150</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I29" s="6">
         <v>4444</v>
@@ -3585,13 +3585,13 @@
         <v>106</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I30" s="6">
         <v>5006</v>
@@ -3671,13 +3671,13 @@
         <v>152</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I31" s="6">
         <v>5257</v>
@@ -3757,13 +3757,13 @@
         <v>48</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I32" s="6">
         <v>4831</v>
@@ -3843,13 +3843,13 @@
         <v>167</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I33" s="6">
         <v>5066</v>
@@ -3929,13 +3929,13 @@
         <v>163</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I34" s="6">
         <v>14888</v>
@@ -4015,13 +4015,13 @@
         <v>143</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I35" s="6">
         <v>4421</v>
@@ -4092,22 +4092,22 @@
         <v>190</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I36" s="6">
         <v>2643</v>
@@ -4187,13 +4187,13 @@
         <v>131</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I37" s="6">
         <v>4519</v>
@@ -4273,13 +4273,13 @@
         <v>112</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I38" s="6">
         <v>5368</v>
@@ -4359,13 +4359,13 @@
         <v>45</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I39" s="6">
         <v>14267</v>
@@ -4445,13 +4445,13 @@
         <v>51</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I40" s="6">
         <v>13647</v>
@@ -4531,13 +4531,13 @@
         <v>154</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I41" s="6">
         <v>9925</v>
@@ -4608,22 +4608,22 @@
         <v>190</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>70</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I42" s="6">
         <v>9305</v>
@@ -4703,13 +4703,13 @@
         <v>148</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I43" s="6">
         <v>9925</v>
@@ -4786,16 +4786,16 @@
         <v>70</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I44" s="6">
         <v>3254</v>
@@ -4875,13 +4875,13 @@
         <v>78</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I45" s="6">
         <v>3964</v>
@@ -4961,13 +4961,13 @@
         <v>182</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I46" s="6">
         <v>16942</v>
@@ -5047,13 +5047,13 @@
         <v>145</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I47" s="6">
         <v>16942</v>
@@ -5133,13 +5133,13 @@
         <v>90</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I48" s="6">
         <v>15508</v>
@@ -5219,13 +5219,13 @@
         <v>173</v>
       </c>
       <c r="F49" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I49" s="6">
         <v>5153</v>
@@ -5305,13 +5305,13 @@
         <v>55</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I50" s="6">
         <v>5162</v>
@@ -5391,13 +5391,13 @@
         <v>184</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I51" s="6">
         <v>5902</v>
@@ -5477,13 +5477,13 @@
         <v>134</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I52" s="6">
         <v>5276</v>
@@ -5563,13 +5563,13 @@
         <v>175</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I53" s="6">
         <v>4240</v>
@@ -5649,13 +5649,13 @@
         <v>186</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I54" s="6">
         <v>5001</v>
@@ -5735,13 +5735,13 @@
         <v>189</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I55" s="6">
         <v>12876</v>
@@ -5821,13 +5821,13 @@
         <v>155</v>
       </c>
       <c r="F56" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I56" s="6">
         <v>3073</v>
@@ -5904,16 +5904,16 @@
         <v>56</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I57" s="6">
         <v>3073</v>
@@ -5993,13 +5993,13 @@
         <v>58</v>
       </c>
       <c r="F58" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I58" s="6">
         <v>4225</v>
@@ -6079,13 +6079,13 @@
         <v>60</v>
       </c>
       <c r="F59" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I59" s="6">
         <v>4033</v>
@@ -6165,13 +6165,13 @@
         <v>125</v>
       </c>
       <c r="F60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I60" s="6">
         <v>5583</v>
@@ -6251,13 +6251,13 @@
         <v>157</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I61" s="6">
         <v>3670</v>
@@ -6337,13 +6337,13 @@
         <v>107</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I62" s="6">
         <v>30283</v>
@@ -6423,13 +6423,13 @@
         <v>117</v>
       </c>
       <c r="F63" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I63" s="6">
         <v>19730</v>
@@ -6509,13 +6509,13 @@
         <v>95</v>
       </c>
       <c r="F64" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I64" s="6">
         <v>21565</v>
@@ -6595,13 +6595,13 @@
         <v>97</v>
       </c>
       <c r="F65" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I65" s="6">
         <v>23401</v>
@@ -6681,13 +6681,13 @@
         <v>99</v>
       </c>
       <c r="F66" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I66" s="6">
         <v>19271</v>
@@ -6767,13 +6767,13 @@
         <v>115</v>
       </c>
       <c r="F67" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H67" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I67" s="6">
         <v>21106</v>
@@ -6853,13 +6853,13 @@
         <v>119</v>
       </c>
       <c r="F68" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H68" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I68" s="6">
         <v>24090</v>
@@ -6939,13 +6939,13 @@
         <v>108</v>
       </c>
       <c r="F69" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H69" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I69" s="6">
         <v>15530</v>
@@ -7025,13 +7025,13 @@
         <v>102</v>
       </c>
       <c r="F70" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H70" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I70" s="6">
         <v>14909</v>
@@ -7111,13 +7111,13 @@
         <v>83</v>
       </c>
       <c r="F71" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H71" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I71" s="6">
         <v>10920</v>
@@ -7197,13 +7197,13 @@
         <v>137</v>
       </c>
       <c r="F72" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I72" s="6">
         <v>68826</v>
@@ -7283,13 +7283,13 @@
         <v>63</v>
       </c>
       <c r="F73" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I73" s="6">
         <v>18528</v>
@@ -7369,13 +7369,13 @@
         <v>65</v>
       </c>
       <c r="F74" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H74" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I74" s="6">
         <v>9847</v>
@@ -7455,13 +7455,13 @@
         <v>91</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H75" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I75" s="6">
         <v>10747</v>
@@ -7541,13 +7541,13 @@
         <v>92</v>
       </c>
       <c r="F76" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H76" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I76" s="6">
         <v>16016</v>
@@ -7627,13 +7627,13 @@
         <v>69</v>
       </c>
       <c r="F77" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H77" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I77" s="6">
         <v>3671</v>
@@ -7713,13 +7713,13 @@
         <v>76</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H78" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I78" s="6">
         <v>4686</v>
@@ -7799,13 +7799,13 @@
         <v>77</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H79" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I79" s="6">
         <v>4818</v>
@@ -7885,13 +7885,13 @@
         <v>177</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H80" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I80" s="6">
         <v>14232</v>
@@ -7971,13 +7971,13 @@
         <v>179</v>
       </c>
       <c r="F81" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H81" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I81" s="6">
         <v>13949</v>
@@ -8057,13 +8057,13 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I82" s="6">
         <v>3424</v>
@@ -8143,13 +8143,13 @@
         <v>104</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H83" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I83" s="6">
         <v>15587</v>
@@ -8220,22 +8220,22 @@
         <v>190</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F84" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H84" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="I84" s="6">
         <v>4449</v>

</xml_diff>